<commit_message>
Voeg de extra velden toe aan het export-scherm
</commit_message>
<xml_diff>
--- a/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
+++ b/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Invulvelden" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Invulvelden!$A$1:$AJ$2</definedName>
     <definedName function="false" hidden="false" name="Agrarisch" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Anders" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="Archeologie" vbProcedure="false">#REF!</definedName>
@@ -777,30 +776,7 @@
     <cellStyle name="Standaard 24" xfId="21"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF5998CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -883,10 +859,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1069,11 +1041,11 @@
   <dimension ref="A1:FF2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="V5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-      <selection pane="topRight" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topRight" activeCell="V2" activeCellId="0" sqref="V2"/>
       <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="3:3"/>
+      <selection pane="bottomRight" activeCell="AD2" activeCellId="0" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1107,7 +1079,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="8" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="8" width="13.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="8" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="1" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="9" width="110.67"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="1" width="20.88"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="1" width="20.44"/>
@@ -1117,7 +1089,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="163" style="8" width="9.11"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="13.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="11" customFormat="true" ht="12" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="n">
         <v>0</v>
       </c>
@@ -1588,10 +1560,9 @@
       <c r="FF2" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ2"/>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3"/>
-    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4"/>
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1600,6 +1571,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Zet de eerste kolommen van het export scherm vast
</commit_message>
<xml_diff>
--- a/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
+++ b/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
@@ -20,54 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Afkorting instantie </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">intern</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Nummer instantie</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> intern</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Kolom evt. voor eigen gebruik</t>
   </si>
@@ -93,53 +46,9 @@
     <t xml:space="preserve">Datering</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Materiaal </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Extra foto's</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Afmetingen </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Plaats</t>
   </si>
   <si>
@@ -152,30 +61,6 @@
     <t xml:space="preserve">Locatie afbeelding</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Taxatiebedrag </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Archiefnr foto</t>
   </si>
   <si>
@@ -191,211 +76,13 @@
     <t xml:space="preserve">Plaatsing op internet</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Catgorie </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Collectie</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Thema </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Stijl </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Google Map</t>
   </si>
   <si>
     <t xml:space="preserve">Bron origineel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creative Commons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kopie van oorspronkelijke omschrijving (veld 06) mét namenlijsten indien aanwezig</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Vergaringvan </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LV = Vergaringdat </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">niet in gebruik bij instelling</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Systeem gegeven </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">intern</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Systeem gegeven </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> intern</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Record aangepast (systeem gegeven)  </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">intern</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -407,7 +94,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -438,39 +125,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="8"/>
-      <color theme="1"/>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="8"/>
-      <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -553,7 +218,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -574,43 +239,43 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -823,7 +488,7 @@
   <dimension ref="A1:FF2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,114 +633,84 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="O2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="P2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="R2" s="9"/>
+      <c r="S2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="T2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="U2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="W2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="X2" s="9"/>
+      <c r="Y2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="AC2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
       <c r="AK2" s="10"/>
       <c r="AL2" s="10"/>
       <c r="AM2" s="10"/>

</xml_diff>

<commit_message>
Punten van de werkgroep verwerkt
</commit_message>
<xml_diff>
--- a/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
+++ b/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
@@ -52,10 +52,10 @@
     <t xml:space="preserve">Plaats</t>
   </si>
   <si>
-    <t xml:space="preserve">Buurtschap/wijk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adres (of locatie)</t>
+    <t xml:space="preserve">Buurt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adres</t>
   </si>
   <si>
     <t xml:space="preserve">Locatie afbeelding</t>
@@ -67,13 +67,13 @@
     <t xml:space="preserve">Archieflocatie</t>
   </si>
   <si>
-    <t xml:space="preserve">Interne opm.</t>
+    <t xml:space="preserve">Opmerking</t>
   </si>
   <si>
     <t xml:space="preserve">Categorie</t>
   </si>
   <si>
-    <t xml:space="preserve">Plaatsing op internet</t>
+    <t xml:space="preserve">Internet</t>
   </si>
   <si>
     <t xml:space="preserve">Collectie</t>
@@ -487,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:FF2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,13 +506,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="1" width="3.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="35.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.05"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="1" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="31.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="44.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="16.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="1" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="1" width="3.51"/>

</xml_diff>

<commit_message>
Standaard cell A:A als geselecteerd
</commit_message>
<xml_diff>
--- a/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
+++ b/Bestandenselektie.HKD/Assets/Excel-invulformulier ZCBS.xlsx
@@ -487,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:FF2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,7 +506,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="1" width="3.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="22.05"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="1" width="3.51"/>

</xml_diff>